<commit_message>
Print Comments, Citation if present
</commit_message>
<xml_diff>
--- a/spec/fixtures/pop_test_sheet_valid.xlsx
+++ b/spec/fixtures/pop_test_sheet_valid.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="333"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
   <si>
     <t>Title Page</t>
   </si>
@@ -296,13 +296,34 @@
   </si>
   <si>
     <t>id: other</t>
+  </si>
+  <si>
+    <t>Comment AP7_F8542p_1773_1</t>
+  </si>
+  <si>
+    <t>Comment AP7_F8542p_1773_2</t>
+  </si>
+  <si>
+    <t>Comment AP7_F8542p_1773_3</t>
+  </si>
+  <si>
+    <t>Comment AP7_F8542p_1773_4</t>
+  </si>
+  <si>
+    <t>Comment AP7_F8542p_1773_5</t>
+  </si>
+  <si>
+    <t>Comment AP7_F8542p_1773_6</t>
+  </si>
+  <si>
+    <t>Comment AP7_F8542p_1773_7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -346,6 +367,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="8">
@@ -438,7 +463,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="78">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -511,6 +536,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -540,7 +568,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="78">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -582,6 +610,9 @@
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -955,10 +986,10 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF1" sqref="AF1"/>
+      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1124,6 +1155,9 @@
       <c r="N2" s="12" t="s">
         <v>53</v>
       </c>
+      <c r="U2" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:32" ht="15.75" customHeight="1">
       <c r="A3" s="12" t="s">
@@ -1159,6 +1193,9 @@
       <c r="N3" s="12" t="s">
         <v>53</v>
       </c>
+      <c r="U3" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" customHeight="1">
       <c r="A4" s="12" t="s">
@@ -1194,6 +1231,9 @@
       <c r="N4" s="12" t="s">
         <v>53</v>
       </c>
+      <c r="U4" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="5" spans="1:32" ht="15.75" customHeight="1">
       <c r="A5" s="12" t="s">
@@ -1229,6 +1269,9 @@
       <c r="N5" s="12" t="s">
         <v>53</v>
       </c>
+      <c r="U5" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:32" ht="15.75" customHeight="1">
       <c r="A6" s="12" t="s">
@@ -1270,6 +1313,9 @@
       <c r="O6" s="12" t="s">
         <v>61</v>
       </c>
+      <c r="U6" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="X6" s="1" t="s">
         <v>46</v>
       </c>
@@ -1317,6 +1363,9 @@
       <c r="Q7" s="1">
         <v>1921</v>
       </c>
+      <c r="U7" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="V7" s="1">
         <v>1921</v>
       </c>
@@ -1360,6 +1409,9 @@
       </c>
       <c r="O8" s="12" t="s">
         <v>63</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="15.75" customHeight="1">
@@ -1407,6 +1459,7 @@
   <sortState ref="A2:AF119">
     <sortCondition ref="A1"/>
   </sortState>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3:B9" r:id="rId1" display="http://franklin.library.upenn.edu/record.html?q=PR2574.P5_1637&amp;id=FRANKLIN_1532581&amp;"/>
     <hyperlink ref="B2" r:id="rId2"/>

</xml_diff>

<commit_message>
Update metadata handling; test
</commit_message>
<xml_diff>
--- a/spec/fixtures/pop_test_sheet_valid.xlsx
+++ b/spec/fixtures/pop_test_sheet_valid.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/GIT/pop_uploader/spec/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="333"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14900" tabRatio="333"/>
   </bookViews>
   <sheets>
     <sheet name="Images for Upload" sheetId="1" r:id="rId1"/>
     <sheet name="Value lists" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -20,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="96">
   <si>
     <t>Title Page</t>
   </si>
@@ -145,21 +153,12 @@
     <t>Spine</t>
   </si>
   <si>
-    <t xml:space="preserve">evidence: associated place </t>
-  </si>
-  <si>
     <t>evidence: transcription</t>
   </si>
   <si>
     <t xml:space="preserve">Head, Tail, Fore Edge </t>
   </si>
   <si>
-    <t>evidence: associated date</t>
-  </si>
-  <si>
-    <t>id: place</t>
-  </si>
-  <si>
     <t>University of Pennsylvania</t>
   </si>
   <si>
@@ -244,42 +243,12 @@
     <t>copy: date of publication</t>
   </si>
   <si>
-    <t>copy: printer/publisher</t>
-  </si>
-  <si>
-    <t>evidence: associated name</t>
-  </si>
-  <si>
-    <t>evidence: description</t>
-  </si>
-  <si>
-    <t>evidence: reference citation</t>
-  </si>
-  <si>
     <t>evidence: comments</t>
   </si>
   <si>
-    <t xml:space="preserve">id: date </t>
-  </si>
-  <si>
     <t>id: owner</t>
   </si>
   <si>
-    <t>id: donor</t>
-  </si>
-  <si>
-    <t>id: recipient</t>
-  </si>
-  <si>
-    <t>id: seller</t>
-  </si>
-  <si>
-    <t>id: selling agent</t>
-  </si>
-  <si>
-    <t>id: buyer</t>
-  </si>
-  <si>
     <t>id: binder</t>
   </si>
   <si>
@@ -317,6 +286,36 @@
   </si>
   <si>
     <t>Comment AP7_F8542p_1773_7</t>
+  </si>
+  <si>
+    <t>copy: current owner</t>
+  </si>
+  <si>
+    <t>copy: current geographic location</t>
+  </si>
+  <si>
+    <t>copy: other id</t>
+  </si>
+  <si>
+    <t>copy: printer/publisher/scribe</t>
+  </si>
+  <si>
+    <t>evidence: date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evidence: place </t>
+  </si>
+  <si>
+    <t>id: librarian</t>
+  </si>
+  <si>
+    <t>id: bookseller/auction house</t>
+  </si>
+  <si>
+    <t>id: role unknown</t>
+  </si>
+  <si>
+    <t>evidence: citation</t>
   </si>
 </sst>
 </file>
@@ -373,7 +372,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,35 +388,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor rgb="FFCFE2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor rgb="FFD9EAD3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor rgb="FFCFE2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor rgb="FFD9D2E9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor rgb="FFD9D2E9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -462,6 +437,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -560,13 +577,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="71" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -659,6 +690,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Value lists"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -983,16 +1031,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
@@ -1023,436 +1071,425 @@
     <col min="30" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15">
+    <row r="1" spans="1:30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="14" t="s">
+      <c r="M1" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="15" t="s">
+      <c r="N1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="O1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="P1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>44</v>
+      <c r="Q1" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="R1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD1" s="1"/>
+    </row>
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1772</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1772</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1772</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1772</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="E6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1772</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1772</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="S7" s="1">
+        <v>1921</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1772</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="U1" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="X1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA1" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB1" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC1" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD1" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE1" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="M9" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="12" t="s">
+      <c r="N9" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1772</v>
+      </c>
+      <c r="Q9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="1">
-        <v>1772</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A3" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1772</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A4" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1772</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A5" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="1">
-        <v>1772</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A6" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1772</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A7" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M7" s="1">
-        <v>1772</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>1921</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="V7" s="1">
-        <v>1921</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M8" s="1">
-        <v>1772</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A9" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M9" s="1">
-        <v>1772</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1">
+    </row>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
     </row>
-    <row r="11" spans="1:32" ht="15.75" customHeight="1">
+    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
     </row>
   </sheetData>
@@ -1468,35 +1505,44 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="6">
+        <x14:dataValidation type="list" allowBlank="1">
+          <x14:formula1>
+            <xm:f>'[1]Value lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>K1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[1]Value lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>L1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>'[1]Value lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>J1</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Value lists'!$E$2:$E$12</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>'Value lists'!$E$2:$E$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>F1</xm:sqref>
+          <xm:sqref>F10:F1048576 J2:J9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>'Value lists'!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>G10:G1048576 K2:K9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>'Value lists'!$C$2:$C$14</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>H10:H1048576 L2:L9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -1510,12 +1556,12 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="5" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
@@ -1527,7 +1573,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1539,7 +1585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
@@ -1551,7 +1597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1563,7 +1609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
@@ -1575,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1587,7 +1633,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
@@ -1599,7 +1645,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
@@ -1611,7 +1657,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1623,7 +1669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>31</v>
       </c>
@@ -1635,7 +1681,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -1647,7 +1693,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
@@ -1656,10 +1702,10 @@
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="C13" s="10" t="s">
         <v>37</v>
@@ -1667,7 +1713,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="C14" s="10" t="s">
         <v>38</v>
@@ -1675,16 +1721,16 @@
       <c r="D14" s="5"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="C17" s="2"/>
       <c r="E17" s="2"/>
@@ -1692,10 +1738,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Handle VIAF links; prepend repository to call number
</commit_message>
<xml_diff>
--- a/spec/fixtures/pop_test_sheet_valid.xlsx
+++ b/spec/fixtures/pop_test_sheet_valid.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
   <si>
     <t>Title Page</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>evidence: citation</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/267632219</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -598,6 +601,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="71"/>
   </cellXfs>
   <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1034,10 +1038,10 @@
   <dimension ref="A1:AD11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1359,6 +1363,9 @@
       <c r="W6" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="AC6" s="20" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
@@ -1500,6 +1507,7 @@
   <hyperlinks>
     <hyperlink ref="B3:B9" r:id="rId1" display="http://franklin.library.upenn.edu/record.html?q=PR2574.P5_1637&amp;id=FRANKLIN_1532581&amp;"/>
     <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="AC6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Remove id_viaf_link from headers.yml
</commit_message>
<xml_diff>
--- a/spec/fixtures/pop_test_sheet_valid.xlsx
+++ b/spec/fixtures/pop_test_sheet_valid.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14900" tabRatio="333"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27240" windowHeight="14900" tabRatio="333"/>
   </bookViews>
   <sheets>
     <sheet name="Images for Upload" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="95">
   <si>
     <t>Title Page</t>
   </si>
@@ -252,9 +252,6 @@
     <t>id: binder</t>
   </si>
   <si>
-    <t>id: viaf authority link</t>
-  </si>
-  <si>
     <t>University of Pennsylvania Libraries</t>
   </si>
   <si>
@@ -316,9 +313,6 @@
   </si>
   <si>
     <t>evidence: citation</t>
-  </si>
-  <si>
-    <t>http://viaf.org/viaf/267632219</t>
   </si>
 </sst>
 </file>
@@ -566,7 +560,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -601,7 +595,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="71"/>
   </cellXfs>
   <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1035,13 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD11"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC6" sqref="AC6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1071,11 +1061,10 @@
     <col min="26" max="26" width="18.5" style="1" customWidth="1"/>
     <col min="27" max="27" width="17.5" style="1" customWidth="1"/>
     <col min="28" max="28" width="22.6640625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="17.33203125" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="14.5" style="1"/>
+    <col min="29" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>62</v>
       </c>
@@ -1095,13 +1084,13 @@
         <v>12</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>87</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>88</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>11</v>
@@ -1125,47 +1114,44 @@
         <v>70</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R1" s="15" t="s">
         <v>41</v>
       </c>
       <c r="S1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>91</v>
       </c>
       <c r="U1" s="16" t="s">
         <v>71</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W1" s="19" t="s">
         <v>72</v>
       </c>
       <c r="X1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" s="18" t="s">
         <v>92</v>
-      </c>
-      <c r="Y1" s="18" t="s">
-        <v>93</v>
       </c>
       <c r="Z1" s="18" t="s">
         <v>73</v>
       </c>
       <c r="AA1" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB1" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC1" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD1" s="1"/>
-    </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="AC1" s="1"/>
+    </row>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>46</v>
       </c>
@@ -1173,7 +1159,7 @@
         <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>45</v>
@@ -1200,10 +1186,10 @@
         <v>50</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>51</v>
       </c>
@@ -1211,7 +1197,7 @@
         <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>45</v>
@@ -1238,10 +1224,10 @@
         <v>50</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>52</v>
       </c>
@@ -1249,7 +1235,7 @@
         <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>45</v>
@@ -1276,10 +1262,10 @@
         <v>50</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>53</v>
       </c>
@@ -1287,7 +1273,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>45</v>
@@ -1314,10 +1300,10 @@
         <v>50</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>54</v>
       </c>
@@ -1325,10 +1311,10 @@
         <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>45</v>
@@ -1358,16 +1344,13 @@
         <v>58</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AC6" s="20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>55</v>
       </c>
@@ -1375,7 +1358,7 @@
         <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>45</v>
@@ -1414,10 +1397,10 @@
         <v>44</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>56</v>
       </c>
@@ -1425,7 +1408,7 @@
         <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>45</v>
@@ -1455,10 +1438,10 @@
         <v>60</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>61</v>
       </c>
@@ -1466,7 +1449,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>45</v>
@@ -1475,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M9" s="12" t="s">
         <v>49</v>
@@ -1493,10 +1476,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
     </row>
-    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
     </row>
   </sheetData>
@@ -1507,7 +1490,6 @@
   <hyperlinks>
     <hyperlink ref="B3:B9" r:id="rId1" display="http://franklin.library.upenn.edu/record.html?q=PR2574.P5_1637&amp;id=FRANKLIN_1532581&amp;"/>
     <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="AC6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>